<commit_message>
info page with template
</commit_message>
<xml_diff>
--- a/src/assets/template.xlsx
+++ b/src/assets/template.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my file\sviluppo\archivio doc\005 - quizonline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my file\sviluppo\FE_2021\quiz\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8589B2E4-08BF-45A4-8195-394CB104B128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B276B1FC-0C3E-43F9-8831-1EE5531A502D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F2B368FB-A76F-4656-A18B-5392C496ABA9}"/>
   </bookViews>
   <sheets>
-    <sheet name="datiquestionario" sheetId="1" r:id="rId1"/>
-    <sheet name="quiz" sheetId="2" r:id="rId2"/>
+    <sheet name="istruzioni" sheetId="3" r:id="rId1"/>
+    <sheet name="datiquestionario" sheetId="1" r:id="rId2"/>
+    <sheet name="quiz" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>CODICE</t>
   </si>
@@ -155,6 +156,51 @@
   </si>
   <si>
     <t>madrid</t>
+  </si>
+  <si>
+    <t>FOGLIO "DATI QUESTIONARIO"</t>
+  </si>
+  <si>
+    <t>FOGLIO "QUIZ"</t>
+  </si>
+  <si>
+    <t>Istruzioni per compliazione del foglio excel</t>
+  </si>
+  <si>
+    <t>Colonna</t>
+  </si>
+  <si>
+    <t>DESCRIZIONE</t>
+  </si>
+  <si>
+    <t>identificativo progressivo della domanda</t>
+  </si>
+  <si>
+    <t>testo delle domanda</t>
+  </si>
+  <si>
+    <t>nella domanda è presente una immagine ? Inserire Si in questo caso, No altrimenti</t>
+  </si>
+  <si>
+    <t>Inserire in questa colonna la risposta corretta</t>
+  </si>
+  <si>
+    <t>inserire in questa colonna la rispsta errata</t>
+  </si>
+  <si>
+    <t>Descrizione del concorso</t>
+  </si>
+  <si>
+    <t>numero delle domande presenti nel foglio "quiz"</t>
+  </si>
+  <si>
+    <t>numero delle risposte ad ogni domanda (valore massimo), se nel concorso ci sono domande con 3 risposte e altre con 4 risposte, inserire 4.</t>
+  </si>
+  <si>
+    <t>colonna delle risposta corretta (lasciare 4)</t>
+  </si>
+  <si>
+    <t>numero di quiz da prendere per la generazione nella simulazione della prova</t>
   </si>
 </sst>
 </file>
@@ -191,7 +237,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,8 +256,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -247,12 +299,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -278,6 +348,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -294,6 +378,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,11 +680,415 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E330B72-FD48-4ED1-9C2E-297BABFDDED2}">
+  <dimension ref="A1:Q21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B20:Q20"/>
+    <mergeCell ref="B21:Q21"/>
+    <mergeCell ref="B14:Q14"/>
+    <mergeCell ref="B15:Q15"/>
+    <mergeCell ref="B16:Q16"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="B18:Q18"/>
+    <mergeCell ref="B19:Q19"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="B8:Q8"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="B10:Q10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4AF887-EFC0-4652-A903-0443CF9C12EC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="150" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView view="pageBreakPreview" zoomScale="150" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,10 +1122,10 @@
         <v>12</v>
       </c>
       <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>4</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -644,16 +1136,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC95FA87-488C-4A31-B5C6-9AB4F5DF24B0}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>